<commit_message>
Adicionado seleção de substatus
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berna\Documents\Phyton\BitrixAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE79DE5-9300-4F52-A8B7-2C28AA81B6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DF3FB0-855D-4577-82D4-06C5F978B51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FC4B1AE4-66FC-48C7-9E9F-918CE71080FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>ICCID</t>
   </si>
@@ -561,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7473D40A-0D8D-493A-A4D7-C72533635F8A}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B17" sqref="B17:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,6 +701,30 @@
         <v>26</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>